<commit_message>
xij loop created not tested
</commit_message>
<xml_diff>
--- a/data/random.xlsx
+++ b/data/random.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="25">
   <si>
     <t>label1</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>rank</t>
   </si>
 </sst>
 </file>
@@ -427,15 +430,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E110"/>
+  <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,8 +454,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>136</v>
       </c>
@@ -468,8 +474,11 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>196</v>
       </c>
@@ -485,8 +494,11 @@
       <c r="E3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>144</v>
       </c>
@@ -502,8 +514,11 @@
       <c r="E4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>133</v>
       </c>
@@ -519,8 +534,11 @@
       <c r="E5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>166</v>
       </c>
@@ -536,8 +554,11 @@
       <c r="E6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>103</v>
       </c>
@@ -553,8 +574,11 @@
       <c r="E7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>161</v>
       </c>
@@ -570,8 +594,11 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>101</v>
       </c>
@@ -587,8 +614,11 @@
       <c r="E9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>194</v>
       </c>
@@ -604,8 +634,11 @@
       <c r="E10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>185</v>
       </c>
@@ -621,8 +654,11 @@
       <c r="E11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>171</v>
       </c>
@@ -638,8 +674,11 @@
       <c r="E12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>125</v>
       </c>
@@ -655,8 +694,11 @@
       <c r="E13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>162</v>
       </c>
@@ -672,8 +714,11 @@
       <c r="E14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>123</v>
       </c>
@@ -689,8 +734,11 @@
       <c r="E15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>160</v>
       </c>
@@ -706,8 +754,11 @@
       <c r="E16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>200</v>
       </c>
@@ -723,8 +774,11 @@
       <c r="E17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>153</v>
       </c>
@@ -740,8 +794,11 @@
       <c r="E18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>188</v>
       </c>
@@ -757,8 +814,11 @@
       <c r="E19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>165</v>
       </c>
@@ -774,8 +834,11 @@
       <c r="E20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>170</v>
       </c>
@@ -791,8 +854,11 @@
       <c r="E21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>108</v>
       </c>
@@ -808,8 +874,11 @@
       <c r="E22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>197</v>
       </c>
@@ -825,8 +894,11 @@
       <c r="E23" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>140</v>
       </c>
@@ -842,8 +914,11 @@
       <c r="E24" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>112</v>
       </c>
@@ -859,8 +934,11 @@
       <c r="E25" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>173</v>
       </c>
@@ -876,8 +954,11 @@
       <c r="E26" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>196</v>
       </c>
@@ -893,8 +974,11 @@
       <c r="E27" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>171</v>
       </c>
@@ -910,8 +994,11 @@
       <c r="E28" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>120</v>
       </c>
@@ -927,8 +1014,11 @@
       <c r="E29" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>122</v>
       </c>
@@ -944,8 +1034,11 @@
       <c r="E30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>131</v>
       </c>
@@ -961,8 +1054,11 @@
       <c r="E31" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>139</v>
       </c>
@@ -978,8 +1074,11 @@
       <c r="E32" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>171</v>
       </c>
@@ -995,8 +1094,11 @@
       <c r="E33" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>138</v>
       </c>
@@ -1012,8 +1114,11 @@
       <c r="E34" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>177</v>
       </c>
@@ -1029,8 +1134,11 @@
       <c r="E35" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>197</v>
       </c>
@@ -1046,8 +1154,11 @@
       <c r="E36" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>185</v>
       </c>
@@ -1063,8 +1174,11 @@
       <c r="E37" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>143</v>
       </c>
@@ -1080,8 +1194,11 @@
       <c r="E38" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>162</v>
       </c>
@@ -1097,8 +1214,11 @@
       <c r="E39" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>154</v>
       </c>
@@ -1114,8 +1234,11 @@
       <c r="E40" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>185</v>
       </c>
@@ -1131,8 +1254,11 @@
       <c r="E41" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>191</v>
       </c>
@@ -1148,8 +1274,11 @@
       <c r="E42" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>145</v>
       </c>
@@ -1165,8 +1294,11 @@
       <c r="E43" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>163</v>
       </c>
@@ -1182,8 +1314,11 @@
       <c r="E44" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>107</v>
       </c>
@@ -1199,8 +1334,11 @@
       <c r="E45" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>168</v>
       </c>
@@ -1216,8 +1354,11 @@
       <c r="E46" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>190</v>
       </c>
@@ -1233,8 +1374,11 @@
       <c r="E47" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>170</v>
       </c>
@@ -1250,8 +1394,11 @@
       <c r="E48" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>156</v>
       </c>
@@ -1267,8 +1414,11 @@
       <c r="E49" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>183</v>
       </c>
@@ -1284,8 +1434,11 @@
       <c r="E50" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>132</v>
       </c>
@@ -1301,8 +1454,11 @@
       <c r="E51" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>126</v>
       </c>
@@ -1318,8 +1474,11 @@
       <c r="E52" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>196</v>
       </c>
@@ -1335,8 +1494,11 @@
       <c r="E53" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>197</v>
       </c>
@@ -1352,8 +1514,11 @@
       <c r="E54" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>110</v>
       </c>
@@ -1369,8 +1534,11 @@
       <c r="E55" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>176</v>
       </c>
@@ -1386,8 +1554,11 @@
       <c r="E56" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>130</v>
       </c>
@@ -1403,8 +1574,11 @@
       <c r="E57" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>114</v>
       </c>
@@ -1420,8 +1594,11 @@
       <c r="E58" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>136</v>
       </c>
@@ -1437,8 +1614,11 @@
       <c r="E59" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>152</v>
       </c>
@@ -1454,8 +1634,11 @@
       <c r="E60" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>193</v>
       </c>
@@ -1471,8 +1654,11 @@
       <c r="E61" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>138</v>
       </c>
@@ -1488,8 +1674,11 @@
       <c r="E62" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>123</v>
       </c>
@@ -1505,8 +1694,11 @@
       <c r="E63" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>191</v>
       </c>
@@ -1522,8 +1714,11 @@
       <c r="E64" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>197</v>
       </c>
@@ -1539,8 +1734,11 @@
       <c r="E65" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>152</v>
       </c>
@@ -1556,8 +1754,11 @@
       <c r="E66" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>108</v>
       </c>
@@ -1573,8 +1774,11 @@
       <c r="E67" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>126</v>
       </c>
@@ -1590,8 +1794,11 @@
       <c r="E68" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>184</v>
       </c>
@@ -1607,8 +1814,11 @@
       <c r="E69" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>112</v>
       </c>
@@ -1624,8 +1834,11 @@
       <c r="E70" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>114</v>
       </c>
@@ -1641,8 +1854,11 @@
       <c r="E71" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>184</v>
       </c>
@@ -1658,8 +1874,11 @@
       <c r="E72" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>153</v>
       </c>
@@ -1675,8 +1894,11 @@
       <c r="E73" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>155</v>
       </c>
@@ -1692,8 +1914,11 @@
       <c r="E74" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>122</v>
       </c>
@@ -1709,8 +1934,11 @@
       <c r="E75" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>192</v>
       </c>
@@ -1726,8 +1954,11 @@
       <c r="E76" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>136</v>
       </c>
@@ -1743,8 +1974,11 @@
       <c r="E77" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>161</v>
       </c>
@@ -1760,8 +1994,11 @@
       <c r="E78" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>172</v>
       </c>
@@ -1777,8 +2014,11 @@
       <c r="E79" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>139</v>
       </c>
@@ -1794,8 +2034,11 @@
       <c r="E80" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>172</v>
       </c>
@@ -1811,8 +2054,11 @@
       <c r="E81" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>107</v>
       </c>
@@ -1828,8 +2074,11 @@
       <c r="E82" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>129</v>
       </c>
@@ -1845,8 +2094,11 @@
       <c r="E83" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>133</v>
       </c>
@@ -1862,8 +2114,11 @@
       <c r="E84" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>195</v>
       </c>
@@ -1879,8 +2134,11 @@
       <c r="E85" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>147</v>
       </c>
@@ -1896,8 +2154,11 @@
       <c r="E86" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>116</v>
       </c>
@@ -1913,8 +2174,11 @@
       <c r="E87" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>120</v>
       </c>
@@ -1930,8 +2194,11 @@
       <c r="E88" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>139</v>
       </c>
@@ -1947,8 +2214,11 @@
       <c r="E89" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>131</v>
       </c>
@@ -1964,8 +2234,11 @@
       <c r="E90" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>172</v>
       </c>
@@ -1981,8 +2254,11 @@
       <c r="E91" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F91">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>122</v>
       </c>
@@ -1998,8 +2274,11 @@
       <c r="E92" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>174</v>
       </c>
@@ -2015,8 +2294,11 @@
       <c r="E93" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F93">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>142</v>
       </c>
@@ -2032,8 +2314,11 @@
       <c r="E94" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F94">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>120</v>
       </c>
@@ -2049,8 +2334,11 @@
       <c r="E95" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>133</v>
       </c>
@@ -2066,8 +2354,11 @@
       <c r="E96" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>197</v>
       </c>
@@ -2083,8 +2374,11 @@
       <c r="E97" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F97">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>188</v>
       </c>
@@ -2100,8 +2394,11 @@
       <c r="E98" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F98">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>140</v>
       </c>
@@ -2117,8 +2414,11 @@
       <c r="E99" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F99">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>154</v>
       </c>
@@ -2134,8 +2434,11 @@
       <c r="E100" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F100">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>168</v>
       </c>
@@ -2151,8 +2454,11 @@
       <c r="E101" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F101">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>127</v>
       </c>
@@ -2168,8 +2474,11 @@
       <c r="E102" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F102">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>120</v>
       </c>
@@ -2185,8 +2494,11 @@
       <c r="E103" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F103">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>111</v>
       </c>
@@ -2202,8 +2514,11 @@
       <c r="E104" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>152</v>
       </c>
@@ -2219,8 +2534,11 @@
       <c r="E105" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F105">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>155</v>
       </c>
@@ -2236,8 +2554,11 @@
       <c r="E106" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F106">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>157</v>
       </c>
@@ -2253,8 +2574,11 @@
       <c r="E107" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F107">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>122</v>
       </c>
@@ -2270,8 +2594,11 @@
       <c r="E108" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F108">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>120</v>
       </c>
@@ -2287,8 +2614,11 @@
       <c r="E109" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>196</v>
       </c>
@@ -2303,6 +2633,9 @@
       </c>
       <c r="E110" t="s">
         <v>15</v>
+      </c>
+      <c r="F110">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
one of four series formed
</commit_message>
<xml_diff>
--- a/data/random.xlsx
+++ b/data/random.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="25">
   <si>
     <t>label1</t>
   </si>
@@ -114,7 +114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -122,13 +122,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2645,24 +2662,641 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>136</v>
+      </c>
+      <c r="B2">
+        <v>291</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1.74</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>196</v>
+      </c>
+      <c r="B3">
+        <v>896</v>
+      </c>
+      <c r="C3">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>144</v>
+      </c>
+      <c r="B4">
+        <v>287</v>
+      </c>
+      <c r="C4">
+        <v>37</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>133</v>
+      </c>
+      <c r="B5">
+        <v>285</v>
+      </c>
+      <c r="C5">
+        <v>38</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>166</v>
+      </c>
+      <c r="B6">
+        <v>392</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>103</v>
+      </c>
+      <c r="B7">
+        <v>494</v>
+      </c>
+      <c r="C7">
+        <v>34</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>136</v>
+      </c>
+      <c r="B8">
+        <v>291</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1.74</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>196</v>
+      </c>
+      <c r="B9">
+        <v>896</v>
+      </c>
+      <c r="C9">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>144</v>
+      </c>
+      <c r="B10">
+        <v>287</v>
+      </c>
+      <c r="C10">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>133</v>
+      </c>
+      <c r="B11">
+        <v>285</v>
+      </c>
+      <c r="C11">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>166</v>
+      </c>
+      <c r="B12">
+        <v>392</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>103</v>
+      </c>
+      <c r="B13">
+        <v>494</v>
+      </c>
+      <c r="C13">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>136</v>
+      </c>
+      <c r="B2" s="2">
+        <v>291</v>
+      </c>
+      <c r="C2" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1.74</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>103</v>
+      </c>
+      <c r="B3" s="2">
+        <v>494</v>
+      </c>
+      <c r="C3" s="2">
+        <v>34</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>136</v>
+      </c>
+      <c r="B4" s="2">
+        <v>291</v>
+      </c>
+      <c r="C4" s="2">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.74</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>103</v>
+      </c>
+      <c r="B5" s="2">
+        <v>494</v>
+      </c>
+      <c r="C5" s="2">
+        <v>34</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>196</v>
+      </c>
+      <c r="B6" s="2">
+        <v>896</v>
+      </c>
+      <c r="C6" s="2">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>166</v>
+      </c>
+      <c r="B7" s="2">
+        <v>392</v>
+      </c>
+      <c r="C7" s="2">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>166</v>
+      </c>
+      <c r="B8" s="2">
+        <v>392</v>
+      </c>
+      <c r="C8" s="2">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>144</v>
+      </c>
+      <c r="B9" s="2">
+        <v>287</v>
+      </c>
+      <c r="C9" s="2">
+        <v>37</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3</v>
+      </c>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>133</v>
+      </c>
+      <c r="B10" s="2">
+        <v>285</v>
+      </c>
+      <c r="C10" s="2">
+        <v>38</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="E10" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>196</v>
+      </c>
+      <c r="B11" s="2">
+        <v>896</v>
+      </c>
+      <c r="C11" s="2">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>144</v>
+      </c>
+      <c r="B12" s="2">
+        <v>287</v>
+      </c>
+      <c r="C12" s="2">
+        <v>37</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="E12" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>133</v>
+      </c>
+      <c r="B13" s="2">
+        <v>285</v>
+      </c>
+      <c r="C13" s="2">
+        <v>38</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="E13" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>196</v>
+      </c>
+      <c r="B16" s="2">
+        <v>896</v>
+      </c>
+      <c r="C16" s="2">
+        <v>18</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>166</v>
+      </c>
+      <c r="B17" s="2">
+        <v>392</v>
+      </c>
+      <c r="C17" s="2">
+        <v>15</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>166</v>
+      </c>
+      <c r="B18" s="2">
+        <v>392</v>
+      </c>
+      <c r="C18" s="2">
+        <v>15</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>144</v>
+      </c>
+      <c r="B19" s="2">
+        <v>287</v>
+      </c>
+      <c r="C19" s="2">
+        <v>37</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="E19" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>133</v>
+      </c>
+      <c r="B20" s="2">
+        <v>285</v>
+      </c>
+      <c r="C20" s="2">
+        <v>38</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="E20" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>196</v>
+      </c>
+      <c r="B21" s="2">
+        <v>896</v>
+      </c>
+      <c r="C21" s="2">
+        <v>18</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E21" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>144</v>
+      </c>
+      <c r="B22" s="2">
+        <v>287</v>
+      </c>
+      <c r="C22" s="2">
+        <v>37</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>133</v>
+      </c>
+      <c r="B23" s="2">
+        <v>285</v>
+      </c>
+      <c r="C23" s="2">
+        <v>38</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="E23" s="2">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>